<commit_message>
pdf to folder experiences improved
</commit_message>
<xml_diff>
--- a/test22.xlsx
+++ b/test22.xlsx
@@ -61,7 +61,7 @@
     <t>['July 2012 ~ present', 'MNAUM International Private Limited, Delhi. (Own', 'Venture)', 'Jan 2011 ~June 2012', 'Oct 1998 ~ Jan 2012', 'Working as Executive Director having business verticals in', 'trading, consultancy and management support.', 'Eaton Group, A US MNC (Industrial/Electrical products)', 'Worked   as   “Country   Controller-India”   as   Group   CFO', 'while   handling   Eleven   Entities   having   5   manufacturing', 'plants, Trading business, Export of Services revenue, BPO,', 'IT Services, International Shares service center and more', 'than 3000 manpower.', 'LG Group in India (USD $120 Billion Conglomerate', 'having World Head Quarter in South Korea)', 'Mar 2004 ~ Jan 2011 Worked as “CFO &amp; Head HR” for LG Life Sciences India', 'Private Limited, a Pharmaceuticals company. The company', 'is   into   trading   business   having   products   under   bio-', 'technology and Export of services.', 'Oct 1998 ~ Feb 2004 Worked   as   “Financial   Controller”   with   LG   Electronics', 'India Private Limited having consumer durables Division', 'and Telecommunication Division. The company is having 2', 'manufacturing   plants,   Trading   business,   revenue   from', 'Services and more than 6000 manpower.', 'Hi-Tech Detergents Limited, a manufacturing plant', 'Apr 1996 ~ Oct 1998', 'for HLL.', 'Worked as Financial Controller with the company, a', 'manufacturing', 'FMCG products like Wheel and Vim Bar.', 'M. Mittal &amp; Co. Chartered Accountants Firm', 'Worked   as   Senior   Consultant   while   Auditing   of   private', 'companies,', 'public   limited,   Government   companies,', 'Income   tax   matters,   arranging   the   credit   facilities   for', 'various type of clients, ROC work etc.', 'Institute of Chartered Accountants of India, Delhi', 'Institute of Cost &amp; Works Accountants of India, Delhi', 'Holding 37th Rank in All India', 'IMT,   Ghaziabad  (Regular   three   years   part-time', 'Sep.91 to Mar 96', 'Certification', '1996    CA', '1995    ICWA', '1997    MBA-Finance', 'course)', 'Academic Credentials', '1991   B.Com.', 'Securing 69.2% marks (86.3% in IIIrd Year) from MMH', 'College, Choudhary Charan Singh University.']</t>
   </si>
   <si>
-    <t>37.33Years</t>
+    <t>23 years</t>
   </si>
   <si>
     <t>Budgeting,Finance,Litigation,Tax,Legal</t>
@@ -432,8 +432,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="9" width="33.7109375" style="1" customWidth="1"/>
-    <col min="11" max="12" width="33.7109375" style="1" customWidth="1"/>
+    <col min="6" max="12" width="33.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -487,7 +486,7 @@
       <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="1" t="s">

</xml_diff>